<commit_message>
update template with comment (#165)
</commit_message>
<xml_diff>
--- a/examples/cmTemplate.xlsx
+++ b/examples/cmTemplate.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="K-Matrix " sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="additionalCollumns" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'K-Matrix '!$A$1:$S$6</definedName>
@@ -22,8 +23,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Starting with this collumn any collumn from table ‚additionalCollumns‘ can be set direct</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -142,6 +167,63 @@
   </si>
   <si>
     <t xml:space="preserve">three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.extended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.isframe_complex_multiplexed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.pgn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame.priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.startBit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.signalsize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.is_little_endian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.is_signed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.multiplex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.mux_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.is_float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.comments</t>
   </si>
 </sst>
 </file>
@@ -245,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +350,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -352,24 +438,24 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S6" activeCellId="0" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.29959514170041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9716599190283"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.29959514170041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="5.29959514170041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.9716599190283"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.8016194331984"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="5.29959514170041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.30364372469636"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.9716599190283"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.336032388664"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.7004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="5.7004048582996"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="5.7004048582996"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.93927125506073"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.080971659919"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.7125506072874"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,5 +773,140 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:B23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7287449392713"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rename findNotUsedBits in get_frame_layout let get_frame_layout create array for each bit containing signals using this bit fix createDummySignals to use  get_frame_layout rename createDummySignals to create_dummy_signals
</commit_message>
<xml_diff>
--- a/examples/cmTemplate.xlsx
+++ b/examples/cmTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="K-Matrix " sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="S1" authorId="0">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">signal.offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.max</t>
   </si>
   <si>
     <t xml:space="preserve">123h</t>
@@ -203,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">signal.min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signal.max</t>
   </si>
   <si>
     <t xml:space="preserve">signal.unit</t>
@@ -433,29 +433,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.93927125506073"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.080971659919"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.7125506072874"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="10" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,13 +519,16 @@
       <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>100</v>
@@ -539,49 +542,52 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>501</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>100</v>
@@ -595,49 +601,49 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>100</v>
@@ -651,49 +657,49 @@
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>100</v>
@@ -707,41 +713,41 @@
         <v>4</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +774,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -784,30 +790,30 @@
   </sheetPr>
   <dimension ref="B3:B23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7287449392713"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,42 +823,42 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,12 +868,12 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +909,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>

<commit_message>
rename findNotUsedBits in get_frame_layout (#254)
* rename findNotUsedBits in get_frame_layout
let get_frame_layout create array for each bit containing signals using this bit
fix createDummySignals to use  get_frame_layout
rename createDummySignals to create_dummy_signals
* store signal (object references) instead of signal names
</commit_message>
<xml_diff>
--- a/examples/cmTemplate.xlsx
+++ b/examples/cmTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="K-Matrix " sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="S1" authorId="0">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">signal.offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal.max</t>
   </si>
   <si>
     <t xml:space="preserve">123h</t>
@@ -203,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">signal.min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signal.max</t>
   </si>
   <si>
     <t xml:space="preserve">signal.unit</t>
@@ -433,29 +433,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="5.7004048582996"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.93927125506073"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.080971659919"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.7125506072874"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="10" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,13 +519,16 @@
       <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>100</v>
@@ -539,49 +542,52 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>501</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>100</v>
@@ -595,49 +601,49 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>100</v>
@@ -651,49 +657,49 @@
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>100</v>
@@ -707,41 +713,41 @@
         <v>4</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +774,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -784,30 +790,30 @@
   </sheetPr>
   <dimension ref="B3:B23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7287449392713"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,42 +823,42 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,12 +868,12 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +909,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>

<commit_message>
import excel template from devbranch
import excel template from devbranch
</commit_message>
<xml_diff>
--- a/examples/cmTemplate.xlsx
+++ b/examples/cmTemplate.xlsx
@@ -435,9 +435,9 @@
   </sheetPr>
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>

</xml_diff>